<commit_message>
sales overview back end
</commit_message>
<xml_diff>
--- a/reference/sales_report/BUDGET_EXIM_2022.xlsx
+++ b/reference/sales_report/BUDGET_EXIM_2022.xlsx
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5565,7 +5565,7 @@
         <v>112</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>3000021121</v>
       </c>
       <c r="E91" t="s">
         <v>121</v>

</xml_diff>